<commit_message>
An - Update README
</commit_message>
<xml_diff>
--- a/REPORT/N2NJS1806_Report0_Mapping.xlsx
+++ b/REPORT/N2NJS1806_Report0_Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22451" windowHeight="9360"/>
+    <workbookView windowWidth="10931" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -703,10 +703,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -755,37 +755,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -805,47 +775,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -868,8 +807,31 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -883,6 +845,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -890,11 +883,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -925,7 +925,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,25 +1009,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,25 +1027,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,7 +1045,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,49 +1069,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,37 +1099,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,17 +1180,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1219,17 +1219,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1251,6 +1260,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1259,38 +1277,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1300,130 +1300,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1782,8 +1782,8 @@
   <sheetPr/>
   <dimension ref="A1:BI85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="BC46" sqref="BC46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="BA16" workbookViewId="0">
+      <selection activeCell="BC49" sqref="BC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2030,7 +2030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" ht="15.15" spans="1:61">
       <c r="A3" s="5" t="s">
         <v>56</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" ht="15.15" spans="1:61">
       <c r="A5" s="5" t="s">
         <v>64</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" ht="15.15" spans="1:61">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" ht="15.15" spans="1:61">
       <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" ht="15.15" spans="1:61">
       <c r="A8" s="5" t="s">
         <v>76</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" ht="15.15" spans="1:61">
       <c r="A9" s="5" t="s">
         <v>80</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" ht="15.15" spans="1:61">
       <c r="A10" s="5" t="s">
         <v>84</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" ht="15.15" spans="1:61">
       <c r="A11" s="5" t="s">
         <v>88</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" ht="15.15" spans="1:61">
       <c r="A13" s="5" t="s">
         <v>96</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" ht="15.15" spans="1:61">
       <c r="A14" s="5" t="s">
         <v>100</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" ht="15.15" spans="1:61">
       <c r="A15" s="5" t="s">
         <v>103</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:61">
+    <row r="17" ht="15.15" spans="1:61">
       <c r="A17" s="5" t="s">
         <v>109</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:61">
+    <row r="18" ht="15.15" spans="1:61">
       <c r="A18" s="5" t="s">
         <v>112</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:61">
+    <row r="19" ht="15.15" spans="1:61">
       <c r="A19" s="5" t="s">
         <v>115</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:61">
+    <row r="20" ht="15.15" spans="1:61">
       <c r="A20" s="5" t="s">
         <v>118</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:61">
+    <row r="21" ht="15.15" spans="1:61">
       <c r="A21" s="5" t="s">
         <v>121</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:61">
+    <row r="22" ht="15.15" spans="1:61">
       <c r="A22" s="5" t="s">
         <v>124</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" ht="15.6" spans="1:61">
+    <row r="23" ht="16.35" spans="1:61">
       <c r="A23" s="5" t="s">
         <v>127</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:61">
+    <row r="24" ht="15.15" spans="1:61">
       <c r="A24" s="5" t="s">
         <v>130</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:61">
+    <row r="25" ht="15.15" spans="1:61">
       <c r="A25" s="5" t="s">
         <v>133</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:61">
+    <row r="26" ht="15.15" spans="1:61">
       <c r="A26" s="5" t="s">
         <v>136</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:61">
+    <row r="27" ht="15.15" spans="1:61">
       <c r="A27" s="5" t="s">
         <v>139</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:61">
+    <row r="28" ht="15.15" spans="1:61">
       <c r="A28" s="5" t="s">
         <v>142</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:61">
+    <row r="29" ht="15.15" spans="1:61">
       <c r="A29" s="5" t="s">
         <v>145</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:61">
+    <row r="30" ht="15.15" spans="1:61">
       <c r="A30" s="5" t="s">
         <v>148</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:61">
+    <row r="31" ht="15.15" spans="1:61">
       <c r="A31" s="5" t="s">
         <v>151</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:61">
+    <row r="34" ht="15.15" spans="1:61">
       <c r="A34" s="5" t="s">
         <v>160</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:61">
+    <row r="35" ht="15.15" spans="1:61">
       <c r="A35" s="5" t="s">
         <v>163</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:61">
+    <row r="36" ht="15.15" spans="1:61">
       <c r="A36" s="5" t="s">
         <v>166</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:61">
+    <row r="37" ht="15.15" spans="1:61">
       <c r="A37" s="5" t="s">
         <v>169</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:61">
+    <row r="38" ht="15.15" spans="1:61">
       <c r="A38" s="5" t="s">
         <v>172</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:61">
+    <row r="39" ht="15.15" spans="1:61">
       <c r="A39" s="5" t="s">
         <v>175</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:61">
+    <row r="40" ht="15.15" spans="1:61">
       <c r="A40" s="5" t="s">
         <v>178</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:61">
+    <row r="41" ht="15.15" spans="1:61">
       <c r="A41" s="5" t="s">
         <v>181</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="1:61">
+    <row r="42" ht="15.15" spans="1:61">
       <c r="A42" s="5" t="s">
         <v>184</v>
       </c>
@@ -4805,6 +4805,7 @@
         <v>186</v>
       </c>
     </row>
+    <row r="44" ht="15.15"/>
     <row r="45" ht="15.15" spans="54:55">
       <c r="BB45" s="8" t="s">
         <v>54</v>
@@ -4813,7 +4814,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" ht="66.75" spans="54:55">
+    <row r="46" ht="53.55" spans="54:55">
       <c r="BB46" s="10">
         <v>1</v>
       </c>

</xml_diff>